<commit_message>
update adnd-adventure-game-book product type
</commit_message>
<xml_diff>
--- a/adnd-adventure-game-book/checklist.xlsx
+++ b/adnd-adventure-game-book/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/adnd-adventure-game-book/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD88EAD-2891-2C48-9477-6F65B0F8CE41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6575915C-D5F5-5D4E-93F4-3EBA41B08A79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="13440" windowHeight="16340" xr2:uid="{A654C372-0B9C-F541-B922-0385DFF864DB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="65">
   <si>
     <t>year</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>1-11</t>
+  </si>
+  <si>
+    <t>slipcase set</t>
   </si>
 </sst>
 </file>
@@ -589,7 +592,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F15" sqref="F15:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -940,7 +943,7 @@
         <v>49</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="G15" s="2"/>
     </row>
@@ -961,7 +964,7 @@
         <v>50</v>
       </c>
       <c r="F16" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="G16" s="2"/>
     </row>
@@ -982,7 +985,7 @@
         <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="G17" s="2"/>
     </row>

</xml_diff>